<commit_message>
abfae23 C03.01.09 - docs(src): Documentation for V4.00.00
Corrections to datasheet
</commit_message>
<xml_diff>
--- a/hardware/boards/axis_portal_v2/docs/Documentation_AP2.xlsx
+++ b/hardware/boards/axis_portal_v2/docs/Documentation_AP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\josep\goldi2\hardware\boards\axis_portal_v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42C8DD7-5170-43D7-B2FD-B74FFE4E3D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F328EEA-D253-4791-A702-93FF6900F27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{28F95597-DC2D-43B8-80C7-4C3F5FC79DF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{28F95597-DC2D-43B8-80C7-4C3F5FC79DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="6" r:id="rId1"/>
@@ -2523,7 +2523,7 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:J14"/>
     </sheetView>
   </sheetViews>
@@ -6570,10 +6570,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6783,7 +6783,7 @@
       <c r="L13" s="126"/>
       <c r="M13" s="126"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="78" t="s">
         <v>313</v>
       </c>
@@ -6861,24 +6861,22 @@
       <c r="M18" s="78"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="126"/>
-      <c r="B19" s="126"/>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
-      <c r="H19" s="126"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="126"/>
-      <c r="K19" s="126"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="78" t="s">
-        <v>314</v>
-      </c>
+      <c r="A20" s="78"/>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
@@ -6893,7 +6891,9 @@
       <c r="M20" s="78"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="78"/>
+      <c r="A21" s="78" t="s">
+        <v>314</v>
+      </c>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
@@ -6983,41 +6983,41 @@
       <c r="M26" s="78"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="78"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="77" t="s">
         <v>275</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="78" t="s">
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="77"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="B28" s="78"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="78"/>
       <c r="B29" s="78"/>
       <c r="C29" s="78"/>
       <c r="D29" s="78"/>
@@ -7047,9 +7047,7 @@
       <c r="M30" s="78"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="78" t="s">
-        <v>315</v>
-      </c>
+      <c r="A31" s="78"/>
       <c r="B31" s="78"/>
       <c r="C31" s="78"/>
       <c r="D31" s="78"/>
@@ -7064,7 +7062,9 @@
       <c r="M31" s="78"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="78"/>
+      <c r="A32" s="78" t="s">
+        <v>315</v>
+      </c>
       <c r="B32" s="78"/>
       <c r="C32" s="78"/>
       <c r="D32" s="78"/>
@@ -7138,16 +7138,30 @@
       <c r="L36" s="78"/>
       <c r="M36" s="78"/>
     </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="78"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="78"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A28:M30"/>
-    <mergeCell ref="A31:M36"/>
+  <mergeCells count="13">
+    <mergeCell ref="A29:M31"/>
+    <mergeCell ref="A32:M37"/>
     <mergeCell ref="A11:M12"/>
     <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A14:M18"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="A20:M26"/>
-    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="A21:M27"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A14:M20"/>
     <mergeCell ref="A10:M10"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>

</xml_diff>